<commit_message>
04 busqueda + pedido
04 busqueda por keuyup + pedido de paletas.
</commit_message>
<xml_diff>
--- a/Angular/Paletas Yahvé.xlsx
+++ b/Angular/Paletas Yahvé.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmedina\Downloads\Curso Angular\Angular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmedina\Downloads\Curso Angular\Angular\Angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5463184E-346D-44E6-A2CD-9FA8C86629FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D7683C-AC48-4A9E-B41F-912716071AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8B9CBAAB-98A8-4499-B93A-25E4DC44FD39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8B9CBAAB-98A8-4499-B93A-25E4DC44FD39}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Venta Paletas Semana 25-28Ago</t>
   </si>
@@ -144,6 +144,30 @@
   </si>
   <si>
     <t>Total Deberia Caja</t>
+  </si>
+  <si>
+    <t>Venta Paletas Semana 28Ago-08Sept</t>
+  </si>
+  <si>
+    <t>V Sandia</t>
+  </si>
+  <si>
+    <t>V Galleta</t>
+  </si>
+  <si>
+    <t>R Naranja</t>
+  </si>
+  <si>
+    <t>R Cacahuate</t>
+  </si>
+  <si>
+    <t>R Mango Verde</t>
+  </si>
+  <si>
+    <t>R Fresa Kiwi</t>
+  </si>
+  <si>
+    <t>NUEVO STOCK SEMANA ENTRANTE</t>
   </si>
 </sst>
 </file>
@@ -208,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -240,12 +264,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -268,6 +303,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -603,21 +650,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734E0C91-4377-4E4F-B8BB-89756185763E}">
-  <dimension ref="B1:N26"/>
+  <dimension ref="B1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N18"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
@@ -1336,7 +1385,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>15</v>
       </c>
@@ -1383,7 +1432,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>16</v>
       </c>
@@ -1430,16 +1479,16 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1467,7 +1516,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1483,7 +1532,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1503,12 +1552,1260 @@
         <v>101.5</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G26" s="5"/>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2">
+        <f>+D28-E28</f>
+        <v>9</v>
+      </c>
+      <c r="G28" s="4">
+        <f>+F28*40</f>
+        <v>360</v>
+      </c>
+      <c r="H28" s="4">
+        <v>25</v>
+      </c>
+      <c r="I28" s="4">
+        <v>40</v>
+      </c>
+      <c r="J28" s="6">
+        <f>+I28-H28</f>
+        <v>15</v>
+      </c>
+      <c r="K28" s="6">
+        <f>+J28*F28</f>
+        <v>135</v>
+      </c>
+      <c r="L28" s="10">
+        <v>10</v>
+      </c>
+      <c r="M28" s="11">
+        <f>+L28-E28</f>
+        <v>-1</v>
+      </c>
+      <c r="N28" s="8">
+        <f>+M28*H28</f>
+        <v>-25</v>
+      </c>
+      <c r="O28">
+        <f>+M28+E28</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" ref="F29:F47" si="8">+D29-E29</f>
+        <v>6</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" ref="G29:G40" si="9">+F29*40</f>
+        <v>240</v>
+      </c>
+      <c r="H29" s="4">
+        <v>25</v>
+      </c>
+      <c r="I29" s="4">
+        <v>40</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" ref="J29:J40" si="10">+I29-H29</f>
+        <v>15</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" ref="K29:K47" si="11">+J29*F29</f>
+        <v>90</v>
+      </c>
+      <c r="L29" s="10">
+        <v>10</v>
+      </c>
+      <c r="M29" s="11">
+        <f t="shared" ref="M29:M47" si="12">+L29-E29</f>
+        <v>6</v>
+      </c>
+      <c r="N29" s="8">
+        <f t="shared" ref="N29:N47" si="13">+M29*H29</f>
+        <v>150</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:O49" si="14">+M29+E29</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2">
+        <v>10</v>
+      </c>
+      <c r="E30" s="2">
+        <v>10</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>25</v>
+      </c>
+      <c r="I30" s="4">
+        <v>40</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="10">
+        <v>10</v>
+      </c>
+      <c r="M30" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="2">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
+      <c r="H31" s="4">
+        <v>25</v>
+      </c>
+      <c r="I31" s="4">
+        <v>40</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="L31" s="10">
+        <v>10</v>
+      </c>
+      <c r="M31" s="11">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="N31" s="8">
+        <f t="shared" si="13"/>
+        <v>125</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="H32" s="4">
+        <v>25</v>
+      </c>
+      <c r="I32" s="4">
+        <v>40</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="L32" s="10">
+        <v>10</v>
+      </c>
+      <c r="M32" s="11">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="N32" s="8">
+        <f t="shared" si="13"/>
+        <v>175</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2">
+        <v>8</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="H33" s="4">
+        <v>25</v>
+      </c>
+      <c r="I33" s="4">
+        <v>40</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="L33" s="10">
+        <v>9</v>
+      </c>
+      <c r="M33" s="11">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="N33" s="8">
+        <f t="shared" si="13"/>
+        <v>25</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="15">
+        <v>7</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="15">
+        <v>9</v>
+      </c>
+      <c r="E34" s="15">
+        <v>7</v>
+      </c>
+      <c r="F34" s="15">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G34" s="16">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="H34" s="16">
+        <v>25</v>
+      </c>
+      <c r="I34" s="16">
+        <v>40</v>
+      </c>
+      <c r="J34" s="17">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K34" s="17">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="L34" s="18">
+        <v>5</v>
+      </c>
+      <c r="M34" s="18">
+        <f t="shared" si="12"/>
+        <v>-2</v>
+      </c>
+      <c r="N34" s="17">
+        <f t="shared" si="13"/>
+        <v>-50</v>
+      </c>
+      <c r="O34" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>8</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2">
+        <v>8</v>
+      </c>
+      <c r="E35" s="2">
+        <v>5</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="9"/>
+        <v>120</v>
+      </c>
+      <c r="H35" s="4">
+        <v>25</v>
+      </c>
+      <c r="I35" s="4">
+        <v>40</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="L35" s="10">
+        <v>8</v>
+      </c>
+      <c r="M35" s="11">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="N35" s="8">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="15">
+        <v>9</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="15">
+        <v>5</v>
+      </c>
+      <c r="E36" s="15">
+        <v>3</v>
+      </c>
+      <c r="F36" s="15">
+        <f t="shared" ref="F36" si="15">+D36-E36</f>
+        <v>2</v>
+      </c>
+      <c r="G36" s="16">
+        <f t="shared" ref="G36" si="16">+F36*40</f>
+        <v>80</v>
+      </c>
+      <c r="H36" s="16">
+        <v>25</v>
+      </c>
+      <c r="I36" s="16">
+        <v>40</v>
+      </c>
+      <c r="J36" s="17">
+        <f t="shared" ref="J36" si="17">+I36-H36</f>
+        <v>15</v>
+      </c>
+      <c r="K36" s="17">
+        <f t="shared" ref="K36" si="18">+J36*F36</f>
+        <v>30</v>
+      </c>
+      <c r="L36" s="18">
+        <v>5</v>
+      </c>
+      <c r="M36" s="18">
+        <f t="shared" ref="M36" si="19">+L36-E36</f>
+        <v>2</v>
+      </c>
+      <c r="N36" s="17">
+        <f t="shared" ref="N36" si="20">+M36*H36</f>
+        <v>50</v>
+      </c>
+      <c r="O36" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
+        <v>10</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="15">
+        <v>5</v>
+      </c>
+      <c r="E37" s="15">
+        <v>3</v>
+      </c>
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F38" si="21">+D37-E37</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <f t="shared" ref="G37:G38" si="22">+F37*40</f>
+        <v>80</v>
+      </c>
+      <c r="H37" s="16">
+        <v>25</v>
+      </c>
+      <c r="I37" s="16">
+        <v>40</v>
+      </c>
+      <c r="J37" s="17">
+        <f t="shared" ref="J37:J38" si="23">+I37-H37</f>
+        <v>15</v>
+      </c>
+      <c r="K37" s="17">
+        <f t="shared" ref="K37:K38" si="24">+J37*F37</f>
+        <v>30</v>
+      </c>
+      <c r="L37" s="18">
+        <v>5</v>
+      </c>
+      <c r="M37" s="18">
+        <f t="shared" ref="M37:M38" si="25">+L37-E37</f>
+        <v>2</v>
+      </c>
+      <c r="N37" s="17">
+        <f t="shared" ref="N37:N38" si="26">+M37*H37</f>
+        <v>50</v>
+      </c>
+      <c r="O37" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="15">
+        <v>11</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="15">
+        <v>0</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0</v>
+      </c>
+      <c r="F38" s="15">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="16">
+        <v>25</v>
+      </c>
+      <c r="I38" s="16">
+        <v>40</v>
+      </c>
+      <c r="J38" s="17">
+        <f t="shared" si="23"/>
+        <v>15</v>
+      </c>
+      <c r="K38" s="17">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="L38" s="18">
+        <v>5</v>
+      </c>
+      <c r="M38" s="18">
+        <f t="shared" si="25"/>
+        <v>5</v>
+      </c>
+      <c r="N38" s="17">
+        <f t="shared" si="26"/>
+        <v>125</v>
+      </c>
+      <c r="O38" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="15">
+        <v>12</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="15">
+        <v>5</v>
+      </c>
+      <c r="E39" s="15">
+        <v>3</v>
+      </c>
+      <c r="F39" s="15">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G39" s="16">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="H39" s="16">
+        <v>25</v>
+      </c>
+      <c r="I39" s="16">
+        <v>40</v>
+      </c>
+      <c r="J39" s="17">
+        <f t="shared" ref="J39" si="27">+I39-H39</f>
+        <v>15</v>
+      </c>
+      <c r="K39" s="17">
+        <f t="shared" ref="K39" si="28">+J39*F39</f>
+        <v>30</v>
+      </c>
+      <c r="L39" s="18">
+        <v>5</v>
+      </c>
+      <c r="M39" s="18">
+        <f t="shared" ref="M39" si="29">+L39-E39</f>
+        <v>2</v>
+      </c>
+      <c r="N39" s="17">
+        <f t="shared" ref="N39" si="30">+M39*H39</f>
+        <v>50</v>
+      </c>
+      <c r="O39" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>13</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="9"/>
+        <v>160</v>
+      </c>
+      <c r="H40" s="4">
+        <v>25</v>
+      </c>
+      <c r="I40" s="4">
+        <v>40</v>
+      </c>
+      <c r="J40" s="6">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="K40" s="6">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="L40" s="10">
+        <v>10</v>
+      </c>
+      <c r="M40" s="11">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="N40" s="8">
+        <f t="shared" si="13"/>
+        <v>250</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="2">
+        <v>10</v>
+      </c>
+      <c r="E41" s="2">
+        <v>6</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="G41" s="4">
+        <f>+F41*23</f>
+        <v>92</v>
+      </c>
+      <c r="H41" s="4">
+        <v>15</v>
+      </c>
+      <c r="I41" s="4">
+        <v>23</v>
+      </c>
+      <c r="J41" s="6">
+        <f>+I41-H41</f>
+        <v>8</v>
+      </c>
+      <c r="K41" s="6">
+        <f t="shared" si="11"/>
+        <v>32</v>
+      </c>
+      <c r="L41" s="10">
+        <v>10</v>
+      </c>
+      <c r="M41" s="11">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="N41" s="8">
+        <f t="shared" si="13"/>
+        <v>60</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>15</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="2">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2">
+        <v>4</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G42" s="4">
+        <f t="shared" ref="G42:G47" si="31">+F42*23</f>
+        <v>23</v>
+      </c>
+      <c r="H42" s="4">
+        <v>15</v>
+      </c>
+      <c r="I42" s="4">
+        <v>23</v>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" ref="J42:J47" si="32">+I42-H42</f>
+        <v>8</v>
+      </c>
+      <c r="K42" s="6">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="L42" s="10">
+        <v>10</v>
+      </c>
+      <c r="M42" s="11">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="N42" s="8">
+        <f t="shared" si="13"/>
+        <v>90</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>16</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="2">
+        <v>10</v>
+      </c>
+      <c r="E43" s="2">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G43" s="4">
+        <f t="shared" si="31"/>
+        <v>69</v>
+      </c>
+      <c r="H43" s="4">
+        <v>15</v>
+      </c>
+      <c r="I43" s="4">
+        <v>23</v>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="32"/>
+        <v>8</v>
+      </c>
+      <c r="K43" s="6">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="L43" s="10">
+        <v>10</v>
+      </c>
+      <c r="M43" s="11">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="N43" s="8">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>17</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="2">
+        <v>5</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G44" s="4">
+        <f t="shared" si="31"/>
+        <v>69</v>
+      </c>
+      <c r="H44" s="4">
+        <v>15</v>
+      </c>
+      <c r="I44" s="4">
+        <v>23</v>
+      </c>
+      <c r="J44" s="6">
+        <f t="shared" si="32"/>
+        <v>8</v>
+      </c>
+      <c r="K44" s="6">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="L44" s="10">
+        <v>10</v>
+      </c>
+      <c r="M44" s="11">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="N44" s="8">
+        <f t="shared" si="13"/>
+        <v>120</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>18</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="2">
+        <v>10</v>
+      </c>
+      <c r="E45" s="2">
+        <v>9</v>
+      </c>
+      <c r="F45" s="2">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" si="31"/>
+        <v>23</v>
+      </c>
+      <c r="H45" s="4">
+        <v>15</v>
+      </c>
+      <c r="I45" s="4">
+        <v>23</v>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="32"/>
+        <v>8</v>
+      </c>
+      <c r="K45" s="6">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="L45" s="10">
+        <v>10</v>
+      </c>
+      <c r="M45" s="11">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="N45" s="8">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="2">
+        <v>10</v>
+      </c>
+      <c r="E46" s="2">
+        <v>7</v>
+      </c>
+      <c r="F46" s="2">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="31"/>
+        <v>69</v>
+      </c>
+      <c r="H46" s="4">
+        <v>15</v>
+      </c>
+      <c r="I46" s="4">
+        <v>23</v>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="32"/>
+        <v>8</v>
+      </c>
+      <c r="K46" s="6">
+        <f t="shared" si="11"/>
+        <v>24</v>
+      </c>
+      <c r="L46" s="10">
+        <v>10</v>
+      </c>
+      <c r="M46" s="11">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="N46" s="8">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>20</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="2">
+        <v>20</v>
+      </c>
+      <c r="E47" s="2">
+        <v>6</v>
+      </c>
+      <c r="F47" s="2">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="G47" s="4">
+        <f t="shared" si="31"/>
+        <v>322</v>
+      </c>
+      <c r="H47" s="4">
+        <v>12</v>
+      </c>
+      <c r="I47" s="4">
+        <v>23</v>
+      </c>
+      <c r="J47" s="6">
+        <f t="shared" si="32"/>
+        <v>11</v>
+      </c>
+      <c r="K47" s="6">
+        <f t="shared" si="11"/>
+        <v>154</v>
+      </c>
+      <c r="L47" s="10">
+        <v>20</v>
+      </c>
+      <c r="M47" s="11">
+        <f t="shared" si="12"/>
+        <v>14</v>
+      </c>
+      <c r="N47" s="8">
+        <f t="shared" si="13"/>
+        <v>168</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>21</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="2">
+        <v>4</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" ref="F48:F49" si="33">+D48-E48</f>
+        <v>1</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" ref="G48:G49" si="34">+F48*23</f>
+        <v>23</v>
+      </c>
+      <c r="H48" s="4">
+        <v>12</v>
+      </c>
+      <c r="I48" s="4">
+        <v>23</v>
+      </c>
+      <c r="J48" s="6">
+        <f t="shared" ref="J48:J49" si="35">+I48-H48</f>
+        <v>11</v>
+      </c>
+      <c r="K48" s="6">
+        <f t="shared" ref="K48:K49" si="36">+J48*F48</f>
+        <v>11</v>
+      </c>
+      <c r="L48" s="10">
+        <v>5</v>
+      </c>
+      <c r="M48" s="11">
+        <f t="shared" ref="M48:M49" si="37">+L48-E48</f>
+        <v>2</v>
+      </c>
+      <c r="N48" s="8">
+        <f t="shared" ref="N48:N49" si="38">+M48*H48</f>
+        <v>24</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <v>22</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" s="2">
+        <v>5</v>
+      </c>
+      <c r="E49" s="2">
+        <v>4</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" si="34"/>
+        <v>23</v>
+      </c>
+      <c r="H49" s="4">
+        <v>12</v>
+      </c>
+      <c r="I49" s="4">
+        <v>23</v>
+      </c>
+      <c r="J49" s="6">
+        <f t="shared" si="35"/>
+        <v>11</v>
+      </c>
+      <c r="K49" s="6">
+        <f t="shared" si="36"/>
+        <v>11</v>
+      </c>
+      <c r="L49" s="10">
+        <v>5</v>
+      </c>
+      <c r="M49" s="11">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="N49" s="8">
+        <f t="shared" si="38"/>
+        <v>12</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G50" s="5"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="3">
+        <f>SUM(D28:D50)</f>
+        <v>179</v>
+      </c>
+      <c r="E55" s="3">
+        <f>SUM(E28:E50)</f>
+        <v>110</v>
+      </c>
+      <c r="F55" s="3">
+        <f>SUM(F28:F50)</f>
+        <v>69</v>
+      </c>
+      <c r="G55" s="3">
+        <f>SUM(G28:G50)</f>
+        <v>2233</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="8">
+        <f>SUM(N28:N50)</f>
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1091</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" s="3">
+        <f>+G55+D56</f>
+        <v>3324</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1715</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="9">
+        <f>SUM(K28:K49)</f>
+        <v>866</v>
+      </c>
+      <c r="H57" s="7">
+        <f>+G57/2</f>
+        <v>433</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
+    <mergeCell ref="B26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>